<commit_message>
Fixed reversion issues with notebook after rebasing to main
</commit_message>
<xml_diff>
--- a/dataframes/CX3_radical_dataframe_input.xlsx
+++ b/dataframes/CX3_radical_dataframe_input.xlsx
@@ -781,40 +781,40 @@
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.00284</v>
+        <v>-0.00034</v>
       </c>
       <c r="H2" t="n">
-        <v>0.124991</v>
+        <v>0.115301</v>
       </c>
       <c r="I2" t="n">
-        <v>0.380713</v>
+        <v>0.404791</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.438148</v>
+        <v>-1.424194</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.7888770000000001</v>
+        <v>-0.7939079999999999</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.112081</v>
+        <v>-0.119445</v>
       </c>
       <c r="M2" t="n">
-        <v>1.480253</v>
+        <v>1.488609</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.731662</v>
+        <v>-0.702527</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.112309</v>
+        <v>-0.121247</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.039265</v>
+        <v>-0.06407499999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.395547</v>
+        <v>1.381135</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.156323</v>
+        <v>-0.164098</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
@@ -889,40 +889,40 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.005387</v>
+        <v>-0.001056</v>
       </c>
       <c r="H3" t="n">
-        <v>0.214866</v>
+        <v>0.201376</v>
       </c>
       <c r="I3" t="n">
-        <v>0.356387</v>
+        <v>0.327991</v>
       </c>
       <c r="J3" t="n">
-        <v>1.47913</v>
+        <v>-1.466329</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.677033</v>
+        <v>-0.707995</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.093803</v>
+        <v>-0.086159</v>
       </c>
       <c r="M3" t="n">
-        <v>-1.443314</v>
+        <v>1.476313</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.727796</v>
+        <v>-0.696708</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.08987000000000001</v>
+        <v>-0.086282</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.041203</v>
+        <v>-0.008926999999999999</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.189963</v>
+        <v>1.203326</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.172714</v>
+        <v>-0.155551</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
@@ -997,40 +997,40 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.103568</v>
+        <v>-0.134053</v>
       </c>
       <c r="H4" t="n">
-        <v>0.004684</v>
+        <v>-0.006085</v>
       </c>
       <c r="I4" t="n">
-        <v>0.359802</v>
+        <v>0.383928</v>
       </c>
       <c r="J4" t="n">
-        <v>1.609306</v>
+        <v>1.582716</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.013421</v>
+        <v>-0.021268</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.09890500000000001</v>
+        <v>-0.098292</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.746864</v>
+        <v>-0.686037</v>
       </c>
       <c r="N4" t="n">
-        <v>-1.106027</v>
+        <v>1.156312</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.129599</v>
+        <v>-0.140988</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.758874</v>
+        <v>-0.762626</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.114765</v>
+        <v>-1.12896</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.131299</v>
+        <v>-0.144648</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -1105,40 +1105,40 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.147767</v>
+        <v>-0.152384</v>
       </c>
       <c r="H5" t="n">
-        <v>0.107689</v>
+        <v>0.116642</v>
       </c>
       <c r="I5" t="n">
-        <v>0.348059</v>
+        <v>0.331493</v>
       </c>
       <c r="J5" t="n">
-        <v>1.547585</v>
+        <v>1.551063</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.230457</v>
+        <v>-0.182631</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.081306</v>
+        <v>-0.077164</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.934026</v>
+        <v>-0.873838</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.925682</v>
+        <v>-0.977083</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.113209</v>
+        <v>-0.10521</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.465792</v>
+        <v>-0.524841</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.048449</v>
+        <v>1.043072</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.153544</v>
+        <v>-0.149119</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -1213,40 +1213,40 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.194958</v>
+        <v>-0.201271</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.006913</v>
+        <v>-0.00366</v>
       </c>
       <c r="I6" t="n">
-        <v>0.319002</v>
+        <v>0.306426</v>
       </c>
       <c r="J6" t="n">
-        <v>1.544501</v>
+        <v>1.53584</v>
       </c>
       <c r="K6" t="n">
-        <v>0.006293</v>
+        <v>-0.052518</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.068979</v>
+        <v>-0.064972</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.682231</v>
+        <v>-0.736148</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.900773</v>
+        <v>-0.878269</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.126527</v>
+        <v>-0.123211</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.667312</v>
+        <v>-0.598421</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.901392</v>
+        <v>0.934446</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.123496</v>
+        <v>-0.118244</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -1349,40 +1349,40 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00791</v>
+        <v>-0.013206</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.002128</v>
+        <v>-0.007764</v>
       </c>
       <c r="I7" t="n">
-        <v>0.339023</v>
+        <v>0.350731</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.678936</v>
+        <v>-0.713704</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.110702</v>
+        <v>-1.095253</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1125</v>
+        <v>-0.120201</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.64202</v>
+        <v>-0.5525060000000001</v>
       </c>
       <c r="N7" t="n">
-        <v>1.131996</v>
+        <v>1.17745</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.111694</v>
+        <v>-0.116697</v>
       </c>
       <c r="P7" t="n">
-        <v>1.313046</v>
+        <v>1.279416</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.019167</v>
+        <v>-0.074433</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.114829</v>
+        <v>-0.113834</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -1457,40 +1457,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.012577</v>
+        <v>0.001751</v>
       </c>
       <c r="H8" t="n">
-        <v>0.088619</v>
+        <v>0.081756</v>
       </c>
       <c r="I8" t="n">
-        <v>0.313161</v>
+        <v>0.335137</v>
       </c>
       <c r="J8" t="n">
-        <v>1.209363</v>
+        <v>-1.108729</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.449069</v>
+        <v>-0.599917</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.098728</v>
+        <v>-0.100082</v>
       </c>
       <c r="M8" t="n">
-        <v>-1.033593</v>
+        <v>1.13139</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.728452</v>
+        <v>-0.568192</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.088812</v>
+        <v>-0.101479</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.188348</v>
+        <v>-0.024411</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.088901</v>
+        <v>1.086353</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.125621</v>
+        <v>-0.133576</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1565,40 +1565,40 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.08106099999999999</v>
+        <v>-0.087673</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.0113</v>
+        <v>0.006346</v>
       </c>
       <c r="I9" t="n">
-        <v>0.310684</v>
+        <v>0.284966</v>
       </c>
       <c r="J9" t="n">
-        <v>1.249372</v>
+        <v>1.241036</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.104675</v>
+        <v>-0.144867</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.085758</v>
+        <v>-0.076769</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.692441</v>
+        <v>-0.449257</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.821865</v>
+        <v>0.970023</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.116776</v>
+        <v>-0.103268</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.47587</v>
+        <v>-0.704106</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.93784</v>
+        <v>-0.831502</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.10815</v>
+        <v>-0.104928</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1673,40 +1673,40 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.006061</v>
+        <v>0.012436</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.004741</v>
+        <v>-0.005935</v>
       </c>
       <c r="I10" t="n">
-        <v>0.286244</v>
+        <v>0.295011</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.88545</v>
+        <v>1.029293</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.550759</v>
+        <v>-0.216279</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.094976</v>
+        <v>-0.101683</v>
       </c>
       <c r="M10" t="n">
-        <v>0.948311</v>
+        <v>-0.714661</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.472567</v>
+        <v>-0.7568049999999999</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.097096</v>
+        <v>-0.097396</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.068922</v>
+        <v>-0.327068</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.028067</v>
+        <v>0.9790180000000001</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.09417200000000001</v>
+        <v>-0.095932</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>

</xml_diff>

<commit_message>
Added environment file and tested jupyter in venv kernel
</commit_message>
<xml_diff>
--- a/dataframes/CX3_radical_dataframe_input.xlsx
+++ b/dataframes/CX3_radical_dataframe_input.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -781,40 +781,40 @@
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.00034</v>
+        <v>0.002679</v>
       </c>
       <c r="H2" t="n">
-        <v>0.115301</v>
+        <v>0.116782</v>
       </c>
       <c r="I2" t="n">
-        <v>0.404791</v>
+        <v>0.419822</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.424194</v>
+        <v>1.4807</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.7939079999999999</v>
+        <v>-0.700134</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.119445</v>
+        <v>-0.125914</v>
       </c>
       <c r="M2" t="n">
-        <v>1.488609</v>
+        <v>-1.425507</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.702527</v>
+        <v>-0.784363</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.121247</v>
+        <v>-0.123064</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.06407499999999999</v>
+        <v>-0.057872</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.381135</v>
+        <v>1.367716</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.164098</v>
+        <v>-0.170843</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
@@ -889,40 +889,40 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.001056</v>
+        <v>0.011203</v>
       </c>
       <c r="H3" t="n">
-        <v>0.201376</v>
+        <v>0.224431</v>
       </c>
       <c r="I3" t="n">
-        <v>0.327991</v>
+        <v>0.346664</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.466329</v>
+        <v>-1.421002</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.707995</v>
+        <v>-0.749111</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.086159</v>
+        <v>-0.084967</v>
       </c>
       <c r="M3" t="n">
-        <v>1.476313</v>
+        <v>1.473656</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.696708</v>
+        <v>-0.6730699999999999</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.086282</v>
+        <v>-0.091923</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.008926999999999999</v>
+        <v>-0.063856</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.203326</v>
+        <v>1.19775</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.155551</v>
+        <v>-0.169773</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
@@ -997,40 +997,40 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.134053</v>
+        <v>-0.129309</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.006085</v>
+        <v>0.00706</v>
       </c>
       <c r="I4" t="n">
-        <v>0.383928</v>
+        <v>0.370343</v>
       </c>
       <c r="J4" t="n">
-        <v>1.582716</v>
+        <v>1.590831</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.021268</v>
+        <v>-0.043715</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.098292</v>
+        <v>-0.095932</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.686037</v>
+        <v>-0.749094</v>
       </c>
       <c r="N4" t="n">
-        <v>1.156312</v>
+        <v>-1.115596</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.140988</v>
+        <v>-0.136415</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.762626</v>
+        <v>-0.712429</v>
       </c>
       <c r="Q4" t="n">
-        <v>-1.12896</v>
+        <v>1.152252</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.144648</v>
+        <v>-0.137996</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -1105,40 +1105,40 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.152384</v>
+        <v>-0.14432</v>
       </c>
       <c r="H5" t="n">
-        <v>0.116642</v>
+        <v>0.09843</v>
       </c>
       <c r="I5" t="n">
-        <v>0.331493</v>
+        <v>0.341551</v>
       </c>
       <c r="J5" t="n">
-        <v>1.551063</v>
+        <v>1.549684</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.182631</v>
+        <v>-0.254352</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.077164</v>
+        <v>-0.080599</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.873838</v>
+        <v>-0.968772</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.977083</v>
+        <v>-0.901166</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.10521</v>
+        <v>-0.113244</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.524841</v>
+        <v>-0.436591</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.043072</v>
+        <v>1.057088</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.149119</v>
+        <v>-0.147709</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -1213,40 +1213,40 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.201271</v>
+        <v>-0.209128</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.00366</v>
+        <v>0.019171</v>
       </c>
       <c r="I6" t="n">
-        <v>0.306426</v>
+        <v>0.327533</v>
       </c>
       <c r="J6" t="n">
-        <v>1.53584</v>
+        <v>1.523963</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.052518</v>
+        <v>-0.192741</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.064972</v>
+        <v>-0.06741800000000001</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.736148</v>
+        <v>-0.537409</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.878269</v>
+        <v>0.978013</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.123211</v>
+        <v>-0.128213</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.598421</v>
+        <v>-0.777426</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.934446</v>
+        <v>-0.804442</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.118244</v>
+        <v>-0.131902</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -1349,40 +1349,40 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.013206</v>
+        <v>0.00177</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.007764</v>
+        <v>0.009312000000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>0.350731</v>
+        <v>0.353032</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.713704</v>
+        <v>-0.662648</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.095253</v>
+        <v>-1.117848</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.120201</v>
+        <v>-0.115516</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.5525060000000001</v>
+        <v>-0.637657</v>
       </c>
       <c r="N7" t="n">
-        <v>1.17745</v>
+        <v>1.127546</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.116697</v>
+        <v>-0.119433</v>
       </c>
       <c r="P7" t="n">
-        <v>1.279416</v>
+        <v>1.298535</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.074433</v>
+        <v>-0.019009</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.113834</v>
+        <v>-0.118083</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -1457,40 +1457,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001751</v>
+        <v>-0.004847</v>
       </c>
       <c r="H8" t="n">
-        <v>0.081756</v>
+        <v>0.08786099999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>0.335137</v>
+        <v>0.333904</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.108729</v>
+        <v>1.16119</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.599917</v>
+        <v>-0.533231</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.100082</v>
+        <v>-0.099868</v>
       </c>
       <c r="M8" t="n">
-        <v>1.13139</v>
+        <v>-1.084401</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.568192</v>
+        <v>-0.647656</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.101479</v>
+        <v>-0.099506</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.024411</v>
+        <v>-0.071941</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.086353</v>
+        <v>1.093026</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.133576</v>
+        <v>-0.13453</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1565,40 +1565,40 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.087673</v>
+        <v>-0.09139600000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>0.006346</v>
+        <v>0.004762</v>
       </c>
       <c r="I9" t="n">
-        <v>0.284966</v>
+        <v>0.312238</v>
       </c>
       <c r="J9" t="n">
-        <v>1.241036</v>
+        <v>1.227146</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.144867</v>
+        <v>-0.047013</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.076769</v>
+        <v>-0.0829</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.449257</v>
+        <v>-0.5911920000000001</v>
       </c>
       <c r="N9" t="n">
-        <v>0.970023</v>
+        <v>-0.884832</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.103268</v>
+        <v>-0.114385</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.704106</v>
+        <v>-0.544558</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.831502</v>
+        <v>0.927084</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.104928</v>
+        <v>-0.114953</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1673,40 +1673,40 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.012436</v>
+        <v>0.010979</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.005935</v>
+        <v>-0.007273</v>
       </c>
       <c r="I10" t="n">
-        <v>0.295011</v>
+        <v>0.277261</v>
       </c>
       <c r="J10" t="n">
-        <v>1.029293</v>
+        <v>1.026126</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.216279</v>
+        <v>-0.237963</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.101683</v>
+        <v>-0.095317</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.714661</v>
+        <v>-0.734105</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.7568049999999999</v>
+        <v>-0.751586</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.097396</v>
+        <v>-0.091922</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.327068</v>
+        <v>-0.303</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.9790180000000001</v>
+        <v>0.996822</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.095932</v>
+        <v>-0.090022</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>

</xml_diff>

<commit_message>
fix paths so that they are cross compatible on windows, max, and linux
</commit_message>
<xml_diff>
--- a/dataframes/CX3_radical_dataframe_input.xlsx
+++ b/dataframes/CX3_radical_dataframe_input.xlsx
@@ -781,40 +781,40 @@
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.002679</v>
+        <v>0.002045</v>
       </c>
       <c r="H2" t="n">
-        <v>0.116782</v>
+        <v>0.12237</v>
       </c>
       <c r="I2" t="n">
-        <v>0.419822</v>
+        <v>0.376024</v>
       </c>
       <c r="J2" t="n">
-        <v>1.4807</v>
+        <v>-1.410655</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.700134</v>
+        <v>-0.824013</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.125914</v>
+        <v>-0.109548</v>
       </c>
       <c r="M2" t="n">
-        <v>-1.425507</v>
+        <v>1.497178</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.784363</v>
+        <v>-0.696792</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.123064</v>
+        <v>-0.112821</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.057872</v>
+        <v>-0.08856799999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.367716</v>
+        <v>1.398434</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.170843</v>
+        <v>-0.153655</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
@@ -889,40 +889,40 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.011203</v>
+        <v>0.008595</v>
       </c>
       <c r="H3" t="n">
-        <v>0.224431</v>
+        <v>0.205328</v>
       </c>
       <c r="I3" t="n">
-        <v>0.346664</v>
+        <v>0.361176</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.421002</v>
+        <v>-1.449752</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.749111</v>
+        <v>-0.710593</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.084967</v>
+        <v>-0.091895</v>
       </c>
       <c r="M3" t="n">
-        <v>1.473656</v>
+        <v>1.471679</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.6730699999999999</v>
+        <v>-0.677548</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.091923</v>
+        <v>-0.096224</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.063856</v>
+        <v>-0.030522</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.19775</v>
+        <v>1.182812</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.169773</v>
+        <v>-0.173057</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
@@ -997,40 +997,40 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.129309</v>
+        <v>-0.131351</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00706</v>
+        <v>-0.007347</v>
       </c>
       <c r="I4" t="n">
-        <v>0.370343</v>
+        <v>0.383419</v>
       </c>
       <c r="J4" t="n">
-        <v>1.590831</v>
+        <v>1.578679</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.043715</v>
+        <v>-0.02453</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.095932</v>
+        <v>-0.098719</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.749094</v>
+        <v>-0.681806</v>
       </c>
       <c r="N4" t="n">
-        <v>-1.115596</v>
+        <v>1.155105</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.136415</v>
+        <v>-0.140171</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.712429</v>
+        <v>-0.765522</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.152252</v>
+        <v>-1.123229</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.137996</v>
+        <v>-0.144528</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -1105,40 +1105,40 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.14432</v>
+        <v>-0.136265</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09843</v>
+        <v>0.104809</v>
       </c>
       <c r="I5" t="n">
-        <v>0.341551</v>
+        <v>0.327248</v>
       </c>
       <c r="J5" t="n">
-        <v>1.549684</v>
+        <v>1.56534</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.254352</v>
+        <v>-0.211146</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.080599</v>
+        <v>-0.079442</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.968772</v>
+        <v>-0.927709</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.901166</v>
+        <v>-0.941207</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.113244</v>
+        <v>-0.104856</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.436591</v>
+        <v>-0.501367</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.057088</v>
+        <v>1.047544</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.147709</v>
+        <v>-0.14295</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -1213,40 +1213,40 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.209128</v>
+        <v>-0.210455</v>
       </c>
       <c r="H6" t="n">
-        <v>0.019171</v>
+        <v>-0.002195</v>
       </c>
       <c r="I6" t="n">
-        <v>0.327533</v>
+        <v>0.335549</v>
       </c>
       <c r="J6" t="n">
-        <v>1.523963</v>
+        <v>1.528302</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.192741</v>
+        <v>0.000402</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.06741800000000001</v>
+        <v>-0.06879300000000001</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.537409</v>
+        <v>-0.673835</v>
       </c>
       <c r="N6" t="n">
-        <v>0.978013</v>
+        <v>0.900729</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.128213</v>
+        <v>-0.132832</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.777426</v>
+        <v>-0.644012</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.804442</v>
+        <v>-0.898936</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.131902</v>
+        <v>-0.133923</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -1349,40 +1349,40 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00177</v>
+        <v>-0.00129</v>
       </c>
       <c r="H7" t="n">
-        <v>0.009312000000000001</v>
+        <v>-0.015968</v>
       </c>
       <c r="I7" t="n">
-        <v>0.353032</v>
+        <v>0.35939</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.662648</v>
+        <v>-0.756426</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.117848</v>
+        <v>-1.06227</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.115516</v>
+        <v>-0.123168</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.637657</v>
+        <v>-0.535283</v>
       </c>
       <c r="N7" t="n">
-        <v>1.127546</v>
+        <v>1.176433</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.119433</v>
+        <v>-0.116348</v>
       </c>
       <c r="P7" t="n">
-        <v>1.298535</v>
+        <v>1.292999</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.019009</v>
+        <v>-0.098195</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.118083</v>
+        <v>-0.119874</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -1457,40 +1457,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.004847</v>
+        <v>0.006274</v>
       </c>
       <c r="H8" t="n">
-        <v>0.08786099999999999</v>
+        <v>0.084373</v>
       </c>
       <c r="I8" t="n">
-        <v>0.333904</v>
+        <v>0.316425</v>
       </c>
       <c r="J8" t="n">
-        <v>1.16119</v>
+        <v>1.206509</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.533231</v>
+        <v>-0.480704</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.099868</v>
+        <v>-0.098214</v>
       </c>
       <c r="M8" t="n">
-        <v>-1.084401</v>
+        <v>-1.06737</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.647656</v>
+        <v>-0.696082</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.099506</v>
+        <v>-0.091955</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.071941</v>
+        <v>-0.145413</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.093026</v>
+        <v>1.092413</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.13453</v>
+        <v>-0.126256</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1565,40 +1565,40 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.09139600000000001</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="H9" t="n">
-        <v>0.004762</v>
+        <v>0.009554999999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>0.312238</v>
+        <v>0.302927</v>
       </c>
       <c r="J9" t="n">
-        <v>1.227146</v>
+        <v>1.245865</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.047013</v>
+        <v>-0.060324</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0829</v>
+        <v>-0.085065</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.5911920000000001</v>
+        <v>-0.629705</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.884832</v>
+        <v>-0.861822</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.114385</v>
+        <v>-0.107614</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.544558</v>
+        <v>-0.54416</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.927084</v>
+        <v>0.912591</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.114953</v>
+        <v>-0.110248</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1673,40 +1673,40 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.010979</v>
+        <v>0.014031</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.007273</v>
+        <v>0.008227999999999999</v>
       </c>
       <c r="I10" t="n">
-        <v>0.277261</v>
+        <v>0.272333</v>
       </c>
       <c r="J10" t="n">
-        <v>1.026126</v>
+        <v>1.04998</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.237963</v>
+        <v>-0.138673</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.095317</v>
+        <v>-0.093754</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.734105</v>
+        <v>-0.630161</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.751586</v>
+        <v>-0.828355</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.091922</v>
+        <v>-0.087287</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.303</v>
+        <v>-0.433849</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.996822</v>
+        <v>0.9588</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.090022</v>
+        <v>-0.091293</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>

</xml_diff>